<commit_message>
Change BG to Black
</commit_message>
<xml_diff>
--- a/Reference/text_Data.xlsx
+++ b/Reference/text_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoonkim/Desktop/02.Web_Design/01.MYRepo/02.LyricsWeb/Reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E489B1-6654-2C48-A183-7A7160E6F72D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546D5B98-0D6D-1747-AF48-BBAE5222907C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4820" yWindow="3680" windowWidth="29780" windowHeight="23140" activeTab="1" xr2:uid="{F15FACF5-BC62-FB4F-B3AB-05A5C185F3DB}"/>
+    <workbookView xWindow="260" yWindow="460" windowWidth="29780" windowHeight="19720" activeTab="1" xr2:uid="{F15FACF5-BC62-FB4F-B3AB-05A5C185F3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="gird" sheetId="3" r:id="rId1"/>
@@ -823,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719623F5-7F7F-794C-8E09-1BD043ED2187}">
   <dimension ref="B1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>